<commit_message>
Creacion de login y secciones
</commit_message>
<xml_diff>
--- a/doc/database/Base de Datos.xlsx
+++ b/doc/database/Base de Datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hundred-my.sharepoint.com/personal/alfredo_benaute_hundred_com_pe/Documents/HUNDRED/PROYECTOS/PERU-CACAO/Ingenieria/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABENAUTE\WORK\GITHUB\PERU-CACAO\smi\doc\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Secciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Secciones!$A$1:$J$30</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -159,6 +160,12 @@
   </si>
   <si>
     <t>Servicios de Estado</t>
+  </si>
+  <si>
+    <t>INSERT INTO `seccion` (`id`, `nombre`, `descripcion`, `idTipoGeoData`, `menuCategoria`, `menuAccion`, `idTipoAccion`, `idSeccionPadre`, `fechaCrea`, `usuarioCrea`, `terminalCrea`, `fechaCambio`, `usuarioCambio`, `terminalCambio`, `activo`, `eliminado`, `created_at`, `updated_at`) VALUES (NULL, 'Cultivos', 'Cultivos', '1', '1', '0', NULL, NULL, '2018-06-29 00:00:00', 'admin', 'local', NULL, NULL, NULL, '1', '0', '2018-06-29 00:00:00', '2018-06-29 00:00:00');</t>
+  </si>
+  <si>
+    <t>NULL, 'Cultivos', 'Cultivos', '1', '1', '0', NULL, NULL, '2018-06-29 00:00:00', 'admin', 'local', NULL, NULL, NULL, '1', '0', '2018-06-29 00:00:00', '2018-06-29 00:00:00'</t>
   </si>
 </sst>
 </file>
@@ -534,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,9 +559,10 @@
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="145" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +593,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -608,8 +619,12 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" t="str">
+        <f>"NULL,'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','"  &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','"  &amp; I2 &amp; "','"  &amp; J2 &amp; "'"</f>
+        <v>NULL,'Cultivos','Cultivos','','1','0','','','1','0'</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -635,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -664,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -693,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -719,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -748,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -777,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -800,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -829,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -858,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -887,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -916,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -945,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -968,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1461,4 +1476,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>